<commit_message>
Salary Report - Debi Check
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateSalary.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateSalary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EA0767-82B1-4C19-955A-00A001658997}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE5CA6A-D709-4232-A247-8DF3D0B08CC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>Employee</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Lead Permission</t>
+  </si>
+  <si>
+    <t>Debi-Check Cancellations</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -441,6 +443,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,7 +785,7 @@
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,45 +854,45 @@
       <c r="B4" s="9"/>
     </row>
     <row r="5" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
     </row>
     <row r="6" spans="1:21" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
     </row>
     <row r="8" spans="1:21" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
@@ -942,6 +945,12 @@
       </c>
       <c r="P9" s="16" t="s">
         <v>49</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -961,6 +970,8 @@
       <c r="N10" s="34"/>
       <c r="O10" s="34"/>
       <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
@@ -1015,6 +1026,14 @@
       </c>
       <c r="P11" s="18">
         <f>SUM(P$10:P10)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="18">
+        <f>SUM(Q$10:Q10)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="18">
+        <f>SUM(R$10:R10)</f>
         <v>0</v>
       </c>
       <c r="U11" s="6">
@@ -1209,24 +1228,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="1:16" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:16" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1246,50 +1265,50 @@
       <c r="L3" s="39"/>
       <c r="M3" s="39"/>
       <c r="N3" s="39"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
     </row>
     <row r="4" spans="1:16" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
     </row>
     <row r="6" spans="1:16" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
     </row>
     <row r="8" spans="1:16" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:16" s="7" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1540,24 +1559,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1576,51 +1595,51 @@
       <c r="K3" s="39"/>
       <c r="L3" s="39"/>
       <c r="M3" s="39"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
     </row>
     <row r="4" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
     </row>
     <row r="6" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
     </row>
     <row r="8" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:16" s="7" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Salary Report DebiCheck Upgrades Template
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateSalary.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateSalary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCA0A004-04C9-4E32-ABFF-808449CB0995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E869368-A11B-4649-8A6C-94D43CC7C94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="598" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="21" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>Employee</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Deb-check Accepted mandates</t>
+  </si>
+  <si>
+    <t>Accepted Mandates</t>
   </si>
 </sst>
 </file>
@@ -788,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -1218,10 +1221,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1238,7 +1241,7 @@
     <col min="16" max="16" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:17" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.85">
       <c r="A1" s="43" t="s">
         <v>30</v>
       </c>
@@ -1255,11 +1258,12 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-    </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:16" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+    </row>
+    <row r="2" spans="1:17" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:17" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="39" t="s">
         <v>5</v>
       </c>
@@ -1279,8 +1283,8 @@
       <c r="O3" s="45"/>
       <c r="P3" s="45"/>
     </row>
-    <row r="4" spans="1:16" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="41" t="s">
         <v>32</v>
       </c>
@@ -1300,8 +1304,8 @@
       <c r="O5" s="45"/>
       <c r="P5" s="45"/>
     </row>
-    <row r="6" spans="1:16" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="7" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="42" t="s">
         <v>31</v>
       </c>
@@ -1321,8 +1325,8 @@
       <c r="O7" s="45"/>
       <c r="P7" s="45"/>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="9" spans="1:16" s="7" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" s="8" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" spans="1:17" s="7" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>0</v>
       </c>
@@ -1371,8 +1375,11 @@
       <c r="P9" s="16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" s="7" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="Q9" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="7" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="4"/>
       <c r="B10" s="22"/>
       <c r="C10" s="24"/>
@@ -1389,8 +1396,9 @@
       <c r="N10" s="22"/>
       <c r="O10" s="34"/>
       <c r="P10" s="34"/>
-    </row>
-    <row r="11" spans="1:16" s="7" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="Q10" s="34"/>
+    </row>
+    <row r="11" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
@@ -1452,8 +1460,12 @@
         <f>SUM(P$10:P10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" s="7" customFormat="1" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="Q11" s="18">
+        <f>SUM(Q$10:Q10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="7" customFormat="1" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -1464,14 +1476,14 @@
       <c r="M12" s="33"/>
       <c r="N12" s="33"/>
     </row>
-    <row r="13" spans="1:16" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="14" spans="1:16" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1531,10 +1543,10 @@
     <sortCondition ref="A3:A38"/>
   </sortState>
   <mergeCells count="4">
-    <mergeCell ref="A1:P1"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A5:P5"/>
     <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="85" fitToWidth="0" orientation="landscape" r:id="rId1"/>

</xml_diff>